<commit_message>
updated user management page
</commit_message>
<xml_diff>
--- a/src/main/resources/files/logins.xlsx
+++ b/src/main/resources/files/logins.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="8580"/>
+    <workbookView windowWidth="23040" windowHeight="8580" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="logins" sheetId="1" r:id="rId1"/>
+    <sheet name="UserDetails" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>Username</t>
   </si>
@@ -38,6 +39,33 @@
   </si>
   <si>
     <t>admin123</t>
+  </si>
+  <si>
+    <t>Andreson</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>anil123</t>
+  </si>
+  <si>
+    <t>EmployeeName</t>
+  </si>
+  <si>
+    <t>Kevin  Mathews</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Enabled</t>
+  </si>
+  <si>
+    <t>UserRole</t>
+  </si>
+  <si>
+    <t>ESS</t>
   </si>
 </sst>
 </file>
@@ -50,14 +78,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -513,148 +534,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -981,7 +1002,7 @@
   <sheetPr/>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -1031,4 +1052,64 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="1"/>
+  <cols>
+    <col min="1" max="1" width="27.5555555555556" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>